<commit_message>
ALL RESULTS ARE READY
</commit_message>
<xml_diff>
--- a/EL.xlsx
+++ b/EL.xlsx
@@ -626,13 +626,13 @@
         <v>1002</v>
       </c>
       <c r="C2">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D2">
         <v>907</v>
       </c>
       <c r="E2">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -652,13 +652,13 @@
         <v>975</v>
       </c>
       <c r="C3">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D3">
         <v>933</v>
       </c>
       <c r="E3">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -678,13 +678,13 @@
         <v>954</v>
       </c>
       <c r="C4">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D4">
         <v>908</v>
       </c>
       <c r="E4">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
@@ -704,7 +704,7 @@
         <v>1055</v>
       </c>
       <c r="C5">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D5">
         <v>979</v>
@@ -730,13 +730,13 @@
         <v>1010</v>
       </c>
       <c r="C6">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="D6">
         <v>996</v>
       </c>
       <c r="E6">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>
@@ -756,13 +756,13 @@
         <v>1073</v>
       </c>
       <c r="C7">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D7">
         <v>1027</v>
       </c>
       <c r="E7">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
@@ -782,13 +782,13 @@
         <v>1034</v>
       </c>
       <c r="C8">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D8">
         <v>967</v>
       </c>
       <c r="E8">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
@@ -808,13 +808,13 @@
         <v>1035</v>
       </c>
       <c r="C9">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D9">
         <v>970</v>
       </c>
       <c r="E9">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
@@ -834,7 +834,7 @@
         <v>1110</v>
       </c>
       <c r="C10">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D10">
         <v>999</v>
@@ -860,13 +860,13 @@
         <v>991</v>
       </c>
       <c r="C11">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D11">
         <v>963</v>
       </c>
       <c r="E11">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F11" t="s">
         <v>7</v>
@@ -886,13 +886,13 @@
         <v>980</v>
       </c>
       <c r="C12">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D12">
         <v>897</v>
       </c>
       <c r="E12">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F12" t="s">
         <v>7</v>
@@ -912,13 +912,13 @@
         <v>1043</v>
       </c>
       <c r="C13">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D13">
         <v>969</v>
       </c>
       <c r="E13">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F13" t="s">
         <v>7</v>
@@ -938,13 +938,13 @@
         <v>1253</v>
       </c>
       <c r="C14">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D14">
         <v>1111</v>
       </c>
       <c r="E14">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="F14" t="s">
         <v>7</v>
@@ -964,13 +964,13 @@
         <v>1045</v>
       </c>
       <c r="C15">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D15">
         <v>966</v>
       </c>
       <c r="E15">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F15" t="s">
         <v>7</v>
@@ -990,13 +990,13 @@
         <v>1047</v>
       </c>
       <c r="C16">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="D16">
         <v>989</v>
       </c>
       <c r="E16">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F16" t="s">
         <v>7</v>
@@ -1016,13 +1016,13 @@
         <v>1061</v>
       </c>
       <c r="C17">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D17">
         <v>991</v>
       </c>
       <c r="E17">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F17" t="s">
         <v>7</v>
@@ -1042,13 +1042,13 @@
         <v>1012</v>
       </c>
       <c r="C18">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D18">
         <v>937</v>
       </c>
       <c r="E18">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
@@ -1068,13 +1068,13 @@
         <v>1104</v>
       </c>
       <c r="C19">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D19">
         <v>1015</v>
       </c>
       <c r="E19">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F19" t="s">
         <v>7</v>
@@ -1094,13 +1094,13 @@
         <v>1118</v>
       </c>
       <c r="C20">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="D20">
         <v>1026</v>
       </c>
       <c r="E20">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F20" t="s">
         <v>7</v>
@@ -1120,13 +1120,13 @@
         <v>944</v>
       </c>
       <c r="C21">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="D21">
         <v>896</v>
       </c>
       <c r="E21">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="F21" t="s">
         <v>7</v>
@@ -4595,7 +4595,7 @@
         <v>15575</v>
       </c>
       <c r="D2">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -4621,7 +4621,7 @@
         <v>15721</v>
       </c>
       <c r="D3">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -4647,7 +4647,7 @@
         <v>15872</v>
       </c>
       <c r="D4">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -4673,10 +4673,10 @@
         <v>16183</v>
       </c>
       <c r="D5">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="E5">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -4699,7 +4699,7 @@
         <v>15615</v>
       </c>
       <c r="D6">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -4725,10 +4725,10 @@
         <v>15744</v>
       </c>
       <c r="D7">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="E7">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
@@ -4751,7 +4751,7 @@
         <v>16226</v>
       </c>
       <c r="D8">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -4777,7 +4777,7 @@
         <v>15994</v>
       </c>
       <c r="D9">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -4803,7 +4803,7 @@
         <v>15799</v>
       </c>
       <c r="D10">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -4829,10 +4829,10 @@
         <v>15903</v>
       </c>
       <c r="D11">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E11">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F11" t="s">
         <v>7</v>
@@ -4855,7 +4855,7 @@
         <v>15911</v>
       </c>
       <c r="D12">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -4881,7 +4881,7 @@
         <v>16275</v>
       </c>
       <c r="D13">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -4907,7 +4907,7 @@
         <v>15732</v>
       </c>
       <c r="D14">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -4933,7 +4933,7 @@
         <v>16005</v>
       </c>
       <c r="D15">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -4959,7 +4959,7 @@
         <v>15852</v>
       </c>
       <c r="D16">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -4985,10 +4985,10 @@
         <v>15728</v>
       </c>
       <c r="D17">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E17">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F17" t="s">
         <v>7</v>
@@ -5011,7 +5011,7 @@
         <v>15938</v>
       </c>
       <c r="D18">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -5037,7 +5037,7 @@
         <v>16082</v>
       </c>
       <c r="D19">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -5063,7 +5063,7 @@
         <v>15597</v>
       </c>
       <c r="D20">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -5089,10 +5089,10 @@
         <v>15669</v>
       </c>
       <c r="D21">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E21">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F21" t="s">
         <v>7</v>
@@ -5148,13 +5148,13 @@
         <v>5930</v>
       </c>
       <c r="C2">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D2">
         <v>5475</v>
       </c>
       <c r="E2">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -5174,13 +5174,13 @@
         <v>6180</v>
       </c>
       <c r="C3">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D3">
         <v>5700</v>
       </c>
       <c r="E3">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -5200,13 +5200,13 @@
         <v>6161</v>
       </c>
       <c r="C4">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D4">
         <v>5649</v>
       </c>
       <c r="E4">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
@@ -5226,13 +5226,13 @@
         <v>6135</v>
       </c>
       <c r="C5">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="D5">
         <v>5682</v>
       </c>
       <c r="E5">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -5252,13 +5252,13 @@
         <v>6396</v>
       </c>
       <c r="C6">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D6">
         <v>5834</v>
       </c>
       <c r="E6">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>
@@ -5278,13 +5278,13 @@
         <v>6029</v>
       </c>
       <c r="C7">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D7">
         <v>5675</v>
       </c>
       <c r="E7">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
@@ -5304,13 +5304,13 @@
         <v>6145</v>
       </c>
       <c r="C8">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D8">
         <v>5667</v>
       </c>
       <c r="E8">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
@@ -5330,13 +5330,13 @@
         <v>6207</v>
       </c>
       <c r="C9">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D9">
         <v>5835</v>
       </c>
       <c r="E9">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
@@ -5356,13 +5356,13 @@
         <v>6092</v>
       </c>
       <c r="C10">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D10">
         <v>5593</v>
       </c>
       <c r="E10">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F10" t="s">
         <v>7</v>
@@ -5382,13 +5382,13 @@
         <v>5987</v>
       </c>
       <c r="C11">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D11">
         <v>5577</v>
       </c>
       <c r="E11">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F11" t="s">
         <v>7</v>
@@ -5408,13 +5408,13 @@
         <v>6000</v>
       </c>
       <c r="C12">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D12">
         <v>5624</v>
       </c>
       <c r="E12">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F12" t="s">
         <v>7</v>
@@ -5434,13 +5434,13 @@
         <v>6096</v>
       </c>
       <c r="C13">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="D13">
         <v>5595</v>
       </c>
       <c r="E13">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F13" t="s">
         <v>7</v>
@@ -5460,13 +5460,13 @@
         <v>5781</v>
       </c>
       <c r="C14">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="D14">
         <v>5470</v>
       </c>
       <c r="E14">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F14" t="s">
         <v>7</v>
@@ -5486,13 +5486,13 @@
         <v>5830</v>
       </c>
       <c r="C15">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D15">
         <v>5414</v>
       </c>
       <c r="E15">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F15" t="s">
         <v>7</v>
@@ -5512,13 +5512,13 @@
         <v>5850</v>
       </c>
       <c r="C16">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="D16">
         <v>5506</v>
       </c>
       <c r="E16">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F16" t="s">
         <v>7</v>
@@ -5538,13 +5538,13 @@
         <v>5968</v>
       </c>
       <c r="C17">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D17">
         <v>5538</v>
       </c>
       <c r="E17">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F17" t="s">
         <v>7</v>
@@ -5564,13 +5564,13 @@
         <v>5628</v>
       </c>
       <c r="C18">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="D18">
         <v>5437</v>
       </c>
       <c r="E18">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
@@ -5590,13 +5590,13 @@
         <v>6307</v>
       </c>
       <c r="C19">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D19">
         <v>5735</v>
       </c>
       <c r="E19">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F19" t="s">
         <v>7</v>
@@ -5616,13 +5616,13 @@
         <v>6049</v>
       </c>
       <c r="C20">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D20">
         <v>5641</v>
       </c>
       <c r="E20">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F20" t="s">
         <v>7</v>
@@ -5642,7 +5642,7 @@
         <v>6229</v>
       </c>
       <c r="C21">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D21">
         <v>5695</v>
@@ -5692,13 +5692,13 @@
         <v>2552</v>
       </c>
       <c r="C2">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="D2">
         <v>2452</v>
       </c>
       <c r="E2">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -5718,7 +5718,7 @@
         <v>2462</v>
       </c>
       <c r="C3">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="D3">
         <v>2422</v>
@@ -5744,7 +5744,7 @@
         <v>2545</v>
       </c>
       <c r="C4">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="D4">
         <v>2512</v>
@@ -5770,7 +5770,7 @@
         <v>2524</v>
       </c>
       <c r="C5">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D5">
         <v>2473</v>
@@ -5796,7 +5796,7 @@
         <v>2474</v>
       </c>
       <c r="C6">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D6">
         <v>2418</v>
@@ -5822,7 +5822,7 @@
         <v>2400</v>
       </c>
       <c r="C7">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="D7">
         <v>2367</v>
@@ -5848,13 +5848,13 @@
         <v>2372</v>
       </c>
       <c r="C8">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="D8">
         <v>2355</v>
       </c>
       <c r="E8">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
@@ -5874,7 +5874,7 @@
         <v>2504</v>
       </c>
       <c r="C9">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="D9">
         <v>2429</v>
@@ -5900,7 +5900,7 @@
         <v>2492</v>
       </c>
       <c r="C10">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="D10">
         <v>2431</v>
@@ -5926,13 +5926,13 @@
         <v>2573</v>
       </c>
       <c r="C11">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D11">
         <v>2480</v>
       </c>
       <c r="E11">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F11" t="s">
         <v>7</v>
@@ -5952,7 +5952,7 @@
         <v>2385</v>
       </c>
       <c r="C12">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="D12">
         <v>2379</v>
@@ -5978,13 +5978,13 @@
         <v>2572</v>
       </c>
       <c r="C13">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="D13">
         <v>2472</v>
       </c>
       <c r="E13">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F13" t="s">
         <v>7</v>
@@ -6004,13 +6004,13 @@
         <v>2488</v>
       </c>
       <c r="C14">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D14">
         <v>2435</v>
       </c>
       <c r="E14">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F14" t="s">
         <v>7</v>
@@ -6030,13 +6030,13 @@
         <v>2540</v>
       </c>
       <c r="C15">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D15">
         <v>2473</v>
       </c>
       <c r="E15">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F15" t="s">
         <v>7</v>
@@ -6056,7 +6056,7 @@
         <v>2491</v>
       </c>
       <c r="C16">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="D16">
         <v>2422</v>
@@ -6082,13 +6082,13 @@
         <v>2451</v>
       </c>
       <c r="C17">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D17">
         <v>2387</v>
       </c>
       <c r="E17">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F17" t="s">
         <v>7</v>
@@ -6108,7 +6108,7 @@
         <v>2459</v>
       </c>
       <c r="C18">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D18">
         <v>2400</v>
@@ -6134,7 +6134,7 @@
         <v>2458</v>
       </c>
       <c r="C19">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="D19">
         <v>2423</v>
@@ -6160,7 +6160,7 @@
         <v>2434</v>
       </c>
       <c r="C20">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="D20">
         <v>2375</v>
@@ -6186,13 +6186,13 @@
         <v>2520</v>
       </c>
       <c r="C21">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="D21">
         <v>2422</v>
       </c>
       <c r="E21">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F21" t="s">
         <v>7</v>
@@ -8300,10 +8300,10 @@
         <v>407</v>
       </c>
       <c r="E2">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="F2">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -8326,10 +8326,10 @@
         <v>499</v>
       </c>
       <c r="E3">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="F3">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
@@ -8352,10 +8352,10 @@
         <v>457</v>
       </c>
       <c r="E4">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="F4">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="G4" t="s">
         <v>7</v>
@@ -8378,10 +8378,10 @@
         <v>478</v>
       </c>
       <c r="E5">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="F5">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
@@ -8404,10 +8404,10 @@
         <v>469</v>
       </c>
       <c r="E6">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="F6">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="G6" t="s">
         <v>7</v>
@@ -8430,10 +8430,10 @@
         <v>453</v>
       </c>
       <c r="E7">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="F7">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="G7" t="s">
         <v>7</v>
@@ -8456,10 +8456,10 @@
         <v>500</v>
       </c>
       <c r="E8">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="F8">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="G8" t="s">
         <v>7</v>
@@ -8482,10 +8482,10 @@
         <v>491</v>
       </c>
       <c r="E9">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F9">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="G9" t="s">
         <v>7</v>
@@ -8508,10 +8508,10 @@
         <v>506</v>
       </c>
       <c r="E10">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="F10">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="G10" t="s">
         <v>7</v>
@@ -8534,10 +8534,10 @@
         <v>513</v>
       </c>
       <c r="E11">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="F11">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="G11" t="s">
         <v>7</v>
@@ -8560,10 +8560,10 @@
         <v>445</v>
       </c>
       <c r="E12">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="F12">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="G12" t="s">
         <v>7</v>
@@ -8586,10 +8586,10 @@
         <v>507</v>
       </c>
       <c r="E13">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="F13">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="G13" t="s">
         <v>7</v>
@@ -8612,10 +8612,10 @@
         <v>608</v>
       </c>
       <c r="E14">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="F14">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="G14" t="s">
         <v>7</v>
@@ -8638,10 +8638,10 @@
         <v>469</v>
       </c>
       <c r="E15">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="F15">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="G15" t="s">
         <v>7</v>
@@ -8664,10 +8664,10 @@
         <v>424</v>
       </c>
       <c r="E16">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="F16">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="G16" t="s">
         <v>7</v>
@@ -8690,10 +8690,10 @@
         <v>529</v>
       </c>
       <c r="E17">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="F17">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="G17" t="s">
         <v>7</v>
@@ -8716,10 +8716,10 @@
         <v>466</v>
       </c>
       <c r="E18">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="F18">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="G18" t="s">
         <v>7</v>
@@ -8742,10 +8742,10 @@
         <v>527</v>
       </c>
       <c r="E19">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="F19">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="G19" t="s">
         <v>7</v>
@@ -8768,10 +8768,10 @@
         <v>566</v>
       </c>
       <c r="E20">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="F20">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="G20" t="s">
         <v>7</v>
@@ -8794,10 +8794,10 @@
         <v>449</v>
       </c>
       <c r="E21">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="F21">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="G21" t="s">
         <v>7</v>
@@ -9538,7 +9538,7 @@
         <v>7707</v>
       </c>
       <c r="D2">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -9564,7 +9564,7 @@
         <v>7766</v>
       </c>
       <c r="D3">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -9590,10 +9590,10 @@
         <v>8144</v>
       </c>
       <c r="D4">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E4">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
@@ -9616,7 +9616,7 @@
         <v>8021</v>
       </c>
       <c r="D5">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -9642,10 +9642,10 @@
         <v>8042</v>
       </c>
       <c r="D6">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E6">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>
@@ -9668,10 +9668,10 @@
         <v>7885</v>
       </c>
       <c r="D7">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="E7">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
@@ -9694,7 +9694,7 @@
         <v>7599</v>
       </c>
       <c r="D8">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -9720,7 +9720,7 @@
         <v>8010</v>
       </c>
       <c r="D9">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -9746,10 +9746,10 @@
         <v>8016</v>
       </c>
       <c r="D10">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E10">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F10" t="s">
         <v>7</v>
@@ -9772,10 +9772,10 @@
         <v>7762</v>
       </c>
       <c r="D11">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E11">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F11" t="s">
         <v>7</v>
@@ -9798,7 +9798,7 @@
         <v>7763</v>
       </c>
       <c r="D12">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -9824,10 +9824,10 @@
         <v>7976</v>
       </c>
       <c r="D13">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="E13">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F13" t="s">
         <v>7</v>
@@ -9850,7 +9850,7 @@
         <v>8069</v>
       </c>
       <c r="D14">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -9876,7 +9876,7 @@
         <v>8154</v>
       </c>
       <c r="D15">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -9902,10 +9902,10 @@
         <v>7992</v>
       </c>
       <c r="D16">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="E16">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F16" t="s">
         <v>7</v>
@@ -9928,7 +9928,7 @@
         <v>8002</v>
       </c>
       <c r="D17">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -9954,10 +9954,10 @@
         <v>7874</v>
       </c>
       <c r="D18">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="E18">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
@@ -9980,7 +9980,7 @@
         <v>7912</v>
       </c>
       <c r="D19">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -10006,7 +10006,7 @@
         <v>7925</v>
       </c>
       <c r="D20">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -10032,10 +10032,10 @@
         <v>7978</v>
       </c>
       <c r="D21">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E21">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F21" t="s">
         <v>7</v>
@@ -10773,13 +10773,13 @@
         <v>6225</v>
       </c>
       <c r="C2">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D2">
         <v>5831</v>
       </c>
       <c r="E2">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -10799,7 +10799,7 @@
         <v>6547</v>
       </c>
       <c r="C3">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D3">
         <v>5816</v>
@@ -10825,13 +10825,13 @@
         <v>6765</v>
       </c>
       <c r="C4">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D4">
         <v>5887</v>
       </c>
       <c r="E4">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
@@ -10851,13 +10851,13 @@
         <v>6036</v>
       </c>
       <c r="C5">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="D5">
         <v>5774</v>
       </c>
       <c r="E5">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -10877,13 +10877,13 @@
         <v>6363</v>
       </c>
       <c r="C6">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D6">
         <v>5989</v>
       </c>
       <c r="E6">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>
@@ -10903,13 +10903,13 @@
         <v>6141</v>
       </c>
       <c r="C7">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="D7">
         <v>5696</v>
       </c>
       <c r="E7">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
@@ -10929,13 +10929,13 @@
         <v>6085</v>
       </c>
       <c r="C8">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D8">
         <v>5854</v>
       </c>
       <c r="E8">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
@@ -10955,13 +10955,13 @@
         <v>6462</v>
       </c>
       <c r="C9">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D9">
         <v>6036</v>
       </c>
       <c r="E9">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
@@ -10981,13 +10981,13 @@
         <v>6238</v>
       </c>
       <c r="C10">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D10">
         <v>5901</v>
       </c>
       <c r="E10">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F10" t="s">
         <v>7</v>
@@ -11007,13 +11007,13 @@
         <v>6559</v>
       </c>
       <c r="C11">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D11">
         <v>6058</v>
       </c>
       <c r="E11">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F11" t="s">
         <v>7</v>
@@ -11033,13 +11033,13 @@
         <v>6308</v>
       </c>
       <c r="C12">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D12">
         <v>5912</v>
       </c>
       <c r="E12">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F12" t="s">
         <v>7</v>
@@ -11059,13 +11059,13 @@
         <v>6990</v>
       </c>
       <c r="C13">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D13">
         <v>5971</v>
       </c>
       <c r="E13">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F13" t="s">
         <v>7</v>
@@ -11085,13 +11085,13 @@
         <v>6832</v>
       </c>
       <c r="C14">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D14">
         <v>6099</v>
       </c>
       <c r="E14">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="F14" t="s">
         <v>7</v>
@@ -11111,13 +11111,13 @@
         <v>6874</v>
       </c>
       <c r="C15">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D15">
         <v>5900</v>
       </c>
       <c r="E15">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F15" t="s">
         <v>7</v>
@@ -11137,13 +11137,13 @@
         <v>6149</v>
       </c>
       <c r="C16">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D16">
         <v>5955</v>
       </c>
       <c r="E16">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="F16" t="s">
         <v>7</v>
@@ -11163,13 +11163,13 @@
         <v>6487</v>
       </c>
       <c r="C17">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D17">
         <v>5760</v>
       </c>
       <c r="E17">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F17" t="s">
         <v>7</v>
@@ -11189,13 +11189,13 @@
         <v>7400</v>
       </c>
       <c r="C18">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D18">
         <v>6230</v>
       </c>
       <c r="E18">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
@@ -11215,13 +11215,13 @@
         <v>6387</v>
       </c>
       <c r="C19">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D19">
         <v>6030</v>
       </c>
       <c r="E19">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F19" t="s">
         <v>7</v>
@@ -11241,7 +11241,7 @@
         <v>6535</v>
       </c>
       <c r="C20">
-        <v>0.264705882352941</v>
+        <v>0.2647058823529412</v>
       </c>
       <c r="D20">
         <v>5867</v>
@@ -11267,13 +11267,13 @@
         <v>6319</v>
       </c>
       <c r="C21">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D21">
         <v>5804</v>
       </c>
       <c r="E21">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F21" t="s">
         <v>7</v>
@@ -11329,7 +11329,7 @@
         <v>3172</v>
       </c>
       <c r="C2">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D2">
         <v>3031</v>
@@ -11355,7 +11355,7 @@
         <v>3134</v>
       </c>
       <c r="C3">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D3">
         <v>3033</v>
@@ -11381,7 +11381,7 @@
         <v>3254</v>
       </c>
       <c r="C4">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D4">
         <v>3103</v>
@@ -11407,7 +11407,7 @@
         <v>3163</v>
       </c>
       <c r="C5">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D5">
         <v>3089</v>
@@ -11433,13 +11433,13 @@
         <v>3121</v>
       </c>
       <c r="C6">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D6">
         <v>2988</v>
       </c>
       <c r="E6">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>
@@ -11459,7 +11459,7 @@
         <v>3054</v>
       </c>
       <c r="C7">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D7">
         <v>2936</v>
@@ -11485,13 +11485,13 @@
         <v>2932</v>
       </c>
       <c r="C8">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D8">
         <v>2879</v>
       </c>
       <c r="E8">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
@@ -11511,13 +11511,13 @@
         <v>3131</v>
       </c>
       <c r="C9">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D9">
         <v>3050</v>
       </c>
       <c r="E9">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
@@ -11537,13 +11537,13 @@
         <v>3137</v>
       </c>
       <c r="C10">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D10">
         <v>3004</v>
       </c>
       <c r="E10">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F10" t="s">
         <v>7</v>
@@ -11563,13 +11563,13 @@
         <v>3313</v>
       </c>
       <c r="C11">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D11">
         <v>3123</v>
       </c>
       <c r="E11">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F11" t="s">
         <v>7</v>
@@ -11589,7 +11589,7 @@
         <v>3045</v>
       </c>
       <c r="C12">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D12">
         <v>2944</v>
@@ -11615,13 +11615,13 @@
         <v>3231</v>
       </c>
       <c r="C13">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D13">
         <v>3089</v>
       </c>
       <c r="E13">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F13" t="s">
         <v>7</v>
@@ -11641,13 +11641,13 @@
         <v>3137</v>
       </c>
       <c r="C14">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D14">
         <v>3012</v>
       </c>
       <c r="E14">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F14" t="s">
         <v>7</v>
@@ -11667,13 +11667,13 @@
         <v>3314</v>
       </c>
       <c r="C15">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D15">
         <v>3181</v>
       </c>
       <c r="E15">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F15" t="s">
         <v>7</v>
@@ -11693,13 +11693,13 @@
         <v>3162</v>
       </c>
       <c r="C16">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D16">
         <v>3025</v>
       </c>
       <c r="E16">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F16" t="s">
         <v>7</v>
@@ -11719,13 +11719,13 @@
         <v>3117</v>
       </c>
       <c r="C17">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D17">
         <v>2982</v>
       </c>
       <c r="E17">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F17" t="s">
         <v>7</v>
@@ -11745,13 +11745,13 @@
         <v>3081</v>
       </c>
       <c r="C18">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D18">
         <v>3006</v>
       </c>
       <c r="E18">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
@@ -11771,7 +11771,7 @@
         <v>3108</v>
       </c>
       <c r="C19">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D19">
         <v>3013</v>
@@ -11797,7 +11797,7 @@
         <v>3164</v>
       </c>
       <c r="C20">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D20">
         <v>3030</v>
@@ -11823,13 +11823,13 @@
         <v>3109</v>
       </c>
       <c r="C21">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D21">
         <v>2962</v>
       </c>
       <c r="E21">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F21" t="s">
         <v>7</v>
@@ -11888,7 +11888,7 @@
         <v>5546</v>
       </c>
       <c r="D2">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -11914,7 +11914,7 @@
         <v>5760</v>
       </c>
       <c r="D3">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -11940,7 +11940,7 @@
         <v>5515</v>
       </c>
       <c r="D4">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -11966,10 +11966,10 @@
         <v>5480</v>
       </c>
       <c r="D5">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="E5">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -11992,7 +11992,7 @@
         <v>5578</v>
       </c>
       <c r="D6">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -12018,7 +12018,7 @@
         <v>5569</v>
       </c>
       <c r="D7">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -12044,10 +12044,10 @@
         <v>5656</v>
       </c>
       <c r="D8">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E8">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
@@ -12070,7 +12070,7 @@
         <v>5520</v>
       </c>
       <c r="D9">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -12096,7 +12096,7 @@
         <v>5594</v>
       </c>
       <c r="D10">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -12122,7 +12122,7 @@
         <v>5541</v>
       </c>
       <c r="D11">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -15591,13 +15591,13 @@
         <v>1990</v>
       </c>
       <c r="C2">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D2">
         <v>1876</v>
       </c>
       <c r="E2">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -15617,13 +15617,13 @@
         <v>1927</v>
       </c>
       <c r="C3">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D3">
         <v>1845</v>
       </c>
       <c r="E3">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -15643,13 +15643,13 @@
         <v>1923</v>
       </c>
       <c r="C4">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D4">
         <v>1864</v>
       </c>
       <c r="E4">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
@@ -15669,13 +15669,13 @@
         <v>2268</v>
       </c>
       <c r="C5">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D5">
         <v>2052</v>
       </c>
       <c r="E5">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -15695,13 +15695,13 @@
         <v>2144</v>
       </c>
       <c r="C6">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D6">
         <v>2071</v>
       </c>
       <c r="E6">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>
@@ -15721,13 +15721,13 @@
         <v>1987</v>
       </c>
       <c r="C7">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D7">
         <v>1950</v>
       </c>
       <c r="E7">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
@@ -15747,13 +15747,13 @@
         <v>2026</v>
       </c>
       <c r="C8">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D8">
         <v>1925</v>
       </c>
       <c r="E8">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
@@ -15773,13 +15773,13 @@
         <v>2221</v>
       </c>
       <c r="C9">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D9">
         <v>2055</v>
       </c>
       <c r="E9">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
@@ -15799,13 +15799,13 @@
         <v>2186</v>
       </c>
       <c r="C10">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D10">
         <v>2070</v>
       </c>
       <c r="E10">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="F10" t="s">
         <v>7</v>
@@ -15825,13 +15825,13 @@
         <v>1992</v>
       </c>
       <c r="C11">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D11">
         <v>1945</v>
       </c>
       <c r="E11">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F11" t="s">
         <v>7</v>
@@ -15851,13 +15851,13 @@
         <v>2094</v>
       </c>
       <c r="C12">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D12">
         <v>1960</v>
       </c>
       <c r="E12">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F12" t="s">
         <v>7</v>
@@ -15877,13 +15877,13 @@
         <v>2126</v>
       </c>
       <c r="C13">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D13">
         <v>1943</v>
       </c>
       <c r="E13">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F13" t="s">
         <v>7</v>
@@ -15903,13 +15903,13 @@
         <v>2270</v>
       </c>
       <c r="C14">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D14">
         <v>2073</v>
       </c>
       <c r="E14">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="F14" t="s">
         <v>7</v>
@@ -15929,13 +15929,13 @@
         <v>2253</v>
       </c>
       <c r="C15">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D15">
         <v>1973</v>
       </c>
       <c r="E15">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="F15" t="s">
         <v>7</v>
@@ -15955,13 +15955,13 @@
         <v>2157</v>
       </c>
       <c r="C16">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D16">
         <v>2029</v>
       </c>
       <c r="E16">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F16" t="s">
         <v>7</v>
@@ -15981,13 +15981,13 @@
         <v>2071</v>
       </c>
       <c r="C17">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D17">
         <v>2021</v>
       </c>
       <c r="E17">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F17" t="s">
         <v>7</v>
@@ -16007,13 +16007,13 @@
         <v>2080</v>
       </c>
       <c r="C18">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D18">
         <v>1895</v>
       </c>
       <c r="E18">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
@@ -16033,7 +16033,7 @@
         <v>2110</v>
       </c>
       <c r="C19">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D19">
         <v>1974</v>
@@ -16059,13 +16059,13 @@
         <v>2139</v>
       </c>
       <c r="C20">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D20">
         <v>2013</v>
       </c>
       <c r="E20">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F20" t="s">
         <v>7</v>
@@ -16085,13 +16085,13 @@
         <v>2118</v>
       </c>
       <c r="C21">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D21">
         <v>1872</v>
       </c>
       <c r="E21">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="F21" t="s">
         <v>7</v>
@@ -18875,13 +18875,13 @@
         <v>2925</v>
       </c>
       <c r="C2">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D2">
         <v>2792</v>
       </c>
       <c r="E2">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -18901,7 +18901,7 @@
         <v>2791</v>
       </c>
       <c r="C3">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="D3">
         <v>2754</v>
@@ -18927,13 +18927,13 @@
         <v>2993</v>
       </c>
       <c r="C4">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D4">
         <v>2938</v>
       </c>
       <c r="E4">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
@@ -18953,7 +18953,7 @@
         <v>2903</v>
       </c>
       <c r="C5">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D5">
         <v>2821</v>
@@ -18979,13 +18979,13 @@
         <v>2854</v>
       </c>
       <c r="C6">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="D6">
         <v>2763</v>
       </c>
       <c r="E6">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>
@@ -19005,7 +19005,7 @@
         <v>2801</v>
       </c>
       <c r="C7">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D7">
         <v>2748</v>
@@ -19031,13 +19031,13 @@
         <v>2688</v>
       </c>
       <c r="C8">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="D8">
         <v>2663</v>
       </c>
       <c r="E8">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
@@ -19057,13 +19057,13 @@
         <v>2916</v>
       </c>
       <c r="C9">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D9">
         <v>2815</v>
       </c>
       <c r="E9">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
@@ -19083,7 +19083,7 @@
         <v>2775</v>
       </c>
       <c r="C10">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="D10">
         <v>2687</v>
@@ -19109,13 +19109,13 @@
         <v>2995</v>
       </c>
       <c r="C11">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D11">
         <v>2870</v>
       </c>
       <c r="E11">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F11" t="s">
         <v>7</v>
@@ -19135,7 +19135,7 @@
         <v>2794</v>
       </c>
       <c r="C12">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D12">
         <v>2744</v>
@@ -19161,13 +19161,13 @@
         <v>2929</v>
       </c>
       <c r="C13">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="D13">
         <v>2820</v>
       </c>
       <c r="E13">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F13" t="s">
         <v>7</v>
@@ -19187,13 +19187,13 @@
         <v>2875</v>
       </c>
       <c r="C14">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D14">
         <v>2788</v>
       </c>
       <c r="E14">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F14" t="s">
         <v>7</v>
@@ -19213,13 +19213,13 @@
         <v>2911</v>
       </c>
       <c r="C15">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D15">
         <v>2829</v>
       </c>
       <c r="E15">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F15" t="s">
         <v>7</v>
@@ -19239,13 +19239,13 @@
         <v>2929</v>
       </c>
       <c r="C16">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D16">
         <v>2800</v>
       </c>
       <c r="E16">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F16" t="s">
         <v>7</v>
@@ -19265,7 +19265,7 @@
         <v>2792</v>
       </c>
       <c r="C17">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D17">
         <v>2720</v>
@@ -19291,13 +19291,13 @@
         <v>2869</v>
       </c>
       <c r="C18">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D18">
         <v>2801</v>
       </c>
       <c r="E18">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
@@ -19317,7 +19317,7 @@
         <v>2858</v>
       </c>
       <c r="C19">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="D19">
         <v>2784</v>
@@ -19343,7 +19343,7 @@
         <v>2854</v>
       </c>
       <c r="C20">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D20">
         <v>2773</v>
@@ -19369,7 +19369,7 @@
         <v>2849</v>
       </c>
       <c r="C21">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="D21">
         <v>2756</v>
@@ -19431,13 +19431,13 @@
         <v>5930</v>
       </c>
       <c r="C2">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D2">
         <v>5475</v>
       </c>
       <c r="E2">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -19457,13 +19457,13 @@
         <v>6180</v>
       </c>
       <c r="C3">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D3">
         <v>5700</v>
       </c>
       <c r="E3">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -19483,13 +19483,13 @@
         <v>6161</v>
       </c>
       <c r="C4">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D4">
         <v>5649</v>
       </c>
       <c r="E4">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
@@ -19509,13 +19509,13 @@
         <v>6135</v>
       </c>
       <c r="C5">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="D5">
         <v>5682</v>
       </c>
       <c r="E5">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -19535,13 +19535,13 @@
         <v>6396</v>
       </c>
       <c r="C6">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D6">
         <v>5834</v>
       </c>
       <c r="E6">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>
@@ -19561,13 +19561,13 @@
         <v>6029</v>
       </c>
       <c r="C7">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D7">
         <v>5675</v>
       </c>
       <c r="E7">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
@@ -19587,13 +19587,13 @@
         <v>6145</v>
       </c>
       <c r="C8">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D8">
         <v>5667</v>
       </c>
       <c r="E8">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
@@ -19613,13 +19613,13 @@
         <v>6207</v>
       </c>
       <c r="C9">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D9">
         <v>5835</v>
       </c>
       <c r="E9">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
@@ -19639,13 +19639,13 @@
         <v>6092</v>
       </c>
       <c r="C10">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D10">
         <v>5593</v>
       </c>
       <c r="E10">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F10" t="s">
         <v>7</v>
@@ -19665,13 +19665,13 @@
         <v>5987</v>
       </c>
       <c r="C11">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D11">
         <v>5577</v>
       </c>
       <c r="E11">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F11" t="s">
         <v>7</v>
@@ -19691,13 +19691,13 @@
         <v>6000</v>
       </c>
       <c r="C12">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D12">
         <v>5624</v>
       </c>
       <c r="E12">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F12" t="s">
         <v>7</v>
@@ -19717,13 +19717,13 @@
         <v>6096</v>
       </c>
       <c r="C13">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="D13">
         <v>5595</v>
       </c>
       <c r="E13">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F13" t="s">
         <v>7</v>
@@ -19743,13 +19743,13 @@
         <v>5781</v>
       </c>
       <c r="C14">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="D14">
         <v>5470</v>
       </c>
       <c r="E14">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F14" t="s">
         <v>7</v>
@@ -19769,13 +19769,13 @@
         <v>5830</v>
       </c>
       <c r="C15">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D15">
         <v>5414</v>
       </c>
       <c r="E15">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F15" t="s">
         <v>7</v>
@@ -19795,13 +19795,13 @@
         <v>5850</v>
       </c>
       <c r="C16">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="D16">
         <v>5506</v>
       </c>
       <c r="E16">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F16" t="s">
         <v>7</v>
@@ -19821,13 +19821,13 @@
         <v>5968</v>
       </c>
       <c r="C17">
-        <v>0.235294117647059</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="D17">
         <v>5538</v>
       </c>
       <c r="E17">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F17" t="s">
         <v>7</v>
@@ -19847,13 +19847,13 @@
         <v>5628</v>
       </c>
       <c r="C18">
-        <v>0.176470588235294</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="D18">
         <v>5437</v>
       </c>
       <c r="E18">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
@@ -19873,13 +19873,13 @@
         <v>6307</v>
       </c>
       <c r="C19">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D19">
         <v>5735</v>
       </c>
       <c r="E19">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F19" t="s">
         <v>7</v>
@@ -19899,13 +19899,13 @@
         <v>6049</v>
       </c>
       <c r="C20">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D20">
         <v>5641</v>
       </c>
       <c r="E20">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="F20" t="s">
         <v>7</v>
@@ -19925,7 +19925,7 @@
         <v>6229</v>
       </c>
       <c r="C21">
-        <v>0.205882352941176</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="D21">
         <v>5695</v>
@@ -19975,13 +19975,13 @@
         <v>3477</v>
       </c>
       <c r="C2">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D2">
         <v>3144</v>
       </c>
       <c r="E2">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -20001,7 +20001,7 @@
         <v>3391</v>
       </c>
       <c r="C3">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D3">
         <v>3097</v>
@@ -20027,7 +20027,7 @@
         <v>3386</v>
       </c>
       <c r="C4">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D4">
         <v>3118</v>
@@ -20053,13 +20053,13 @@
         <v>3497</v>
       </c>
       <c r="C5">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D5">
         <v>3176</v>
       </c>
       <c r="E5">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -20079,7 +20079,7 @@
         <v>3563</v>
       </c>
       <c r="C6">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D6">
         <v>3237</v>
@@ -20105,13 +20105,13 @@
         <v>3161</v>
       </c>
       <c r="C7">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D7">
         <v>2994</v>
       </c>
       <c r="E7">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
@@ -20131,13 +20131,13 @@
         <v>3553</v>
       </c>
       <c r="C8">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D8">
         <v>3249</v>
       </c>
       <c r="E8">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
@@ -20157,13 +20157,13 @@
         <v>3557</v>
       </c>
       <c r="C9">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D9">
         <v>3212</v>
       </c>
       <c r="E9">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
@@ -20183,13 +20183,13 @@
         <v>3282</v>
       </c>
       <c r="C10">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D10">
         <v>2990</v>
       </c>
       <c r="E10">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F10" t="s">
         <v>7</v>
@@ -20209,7 +20209,7 @@
         <v>3592</v>
       </c>
       <c r="C11">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D11">
         <v>3241</v>
@@ -20235,13 +20235,13 @@
         <v>3204</v>
       </c>
       <c r="C12">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D12">
         <v>3136</v>
       </c>
       <c r="E12">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F12" t="s">
         <v>7</v>
@@ -20261,13 +20261,13 @@
         <v>3331</v>
       </c>
       <c r="C13">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D13">
         <v>3247</v>
       </c>
       <c r="E13">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F13" t="s">
         <v>7</v>
@@ -20287,13 +20287,13 @@
         <v>3282</v>
       </c>
       <c r="C14">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D14">
         <v>3178</v>
       </c>
       <c r="E14">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F14" t="s">
         <v>7</v>
@@ -20313,13 +20313,13 @@
         <v>3541</v>
       </c>
       <c r="C15">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D15">
         <v>3158</v>
       </c>
       <c r="E15">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F15" t="s">
         <v>7</v>
@@ -20339,13 +20339,13 @@
         <v>3405</v>
       </c>
       <c r="C16">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D16">
         <v>3085</v>
       </c>
       <c r="E16">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F16" t="s">
         <v>7</v>
@@ -20365,7 +20365,7 @@
         <v>3564</v>
       </c>
       <c r="C17">
-        <v>0.08823529411764711</v>
+        <v>0.08823529411764706</v>
       </c>
       <c r="D17">
         <v>3228</v>
@@ -20391,13 +20391,13 @@
         <v>3335</v>
       </c>
       <c r="C18">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D18">
         <v>3093</v>
       </c>
       <c r="E18">
-        <v>0.0588235294117647</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
@@ -20417,13 +20417,13 @@
         <v>3396</v>
       </c>
       <c r="C19">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D19">
         <v>3331</v>
       </c>
       <c r="E19">
-        <v>0.0294117647058824</v>
+        <v>0.02941176470588236</v>
       </c>
       <c r="F19" t="s">
         <v>7</v>
@@ -20443,7 +20443,7 @@
         <v>3429</v>
       </c>
       <c r="C20">
-        <v>0.117647058823529</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="D20">
         <v>3117</v>
@@ -20469,7 +20469,7 @@
         <v>3372</v>
       </c>
       <c r="C21">
-        <v>0.147058823529412</v>
+        <v>0.1470588235294117</v>
       </c>
       <c r="D21">
         <v>3091</v>

</xml_diff>